<commit_message>
Fig 2 data extracted
</commit_message>
<xml_diff>
--- a/New costs.xlsx
+++ b/New costs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\ESM-Italy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6653C129-B10C-4702-BCBC-7E14B3F99458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE75DC0-9D8E-4500-839F-12357A695AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="electrolyzers" sheetId="1" r:id="rId1"/>
+    <sheet name="PV" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,9 +37,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="34">
   <si>
     <t>new value</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>T13</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>T17</t>
+  </si>
+  <si>
+    <t>T18</t>
+  </si>
+  <si>
+    <t>T19</t>
+  </si>
+  <si>
+    <t>T20</t>
+  </si>
+  <si>
+    <t>T21</t>
+  </si>
+  <si>
+    <t>T22</t>
+  </si>
+  <si>
+    <t>T23</t>
+  </si>
+  <si>
+    <t>T24</t>
+  </si>
+  <si>
+    <t>T25</t>
+  </si>
+  <si>
+    <t>T26</t>
+  </si>
+  <si>
+    <t>T27</t>
+  </si>
+  <si>
+    <t>T28</t>
+  </si>
+  <si>
+    <t>T29</t>
+  </si>
+  <si>
+    <t>T30</t>
+  </si>
+  <si>
+    <t>T31</t>
+  </si>
+  <si>
+    <t>T32</t>
+  </si>
+  <si>
+    <t>T33</t>
   </si>
 </sst>
 </file>
@@ -74,8 +174,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,18 +459,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1990</v>
       </c>
@@ -377,7 +478,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1991</v>
       </c>
@@ -385,7 +486,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1992</v>
       </c>
@@ -393,7 +494,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1993</v>
       </c>
@@ -401,7 +502,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1994</v>
       </c>
@@ -409,7 +510,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1995</v>
       </c>
@@ -417,7 +518,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1996</v>
       </c>
@@ -425,7 +526,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1997</v>
       </c>
@@ -433,7 +534,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1998</v>
       </c>
@@ -441,7 +542,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1999</v>
       </c>
@@ -449,7 +550,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2000</v>
       </c>
@@ -457,7 +558,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2001</v>
       </c>
@@ -465,7 +566,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2002</v>
       </c>
@@ -473,7 +574,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2003</v>
       </c>
@@ -481,7 +582,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2004</v>
       </c>
@@ -489,7 +590,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2005</v>
       </c>
@@ -497,7 +598,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2006</v>
       </c>
@@ -505,7 +606,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2007</v>
       </c>
@@ -513,7 +614,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2008</v>
       </c>
@@ -521,7 +622,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2009</v>
       </c>
@@ -529,7 +630,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2010</v>
       </c>
@@ -537,7 +638,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2011</v>
       </c>
@@ -545,7 +646,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2012</v>
       </c>
@@ -553,7 +654,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2013</v>
       </c>
@@ -561,7 +662,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2014</v>
       </c>
@@ -569,7 +670,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2015</v>
       </c>
@@ -577,7 +678,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2016</v>
       </c>
@@ -585,7 +686,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2017</v>
       </c>
@@ -593,7 +694,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2018</v>
       </c>
@@ -601,7 +702,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -609,7 +710,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -617,7 +718,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2021</v>
       </c>
@@ -625,7 +726,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2022</v>
       </c>
@@ -633,7 +734,7 @@
         <v>764912.28070175438</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2023</v>
       </c>
@@ -642,7 +743,7 @@
         <v>746021.30325814534</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2024</v>
       </c>
@@ -651,7 +752,7 @@
         <v>727130.32581453631</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2025</v>
       </c>
@@ -660,7 +761,7 @@
         <v>708239.34837092727</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2026</v>
       </c>
@@ -669,7 +770,7 @@
         <v>689348.37092731823</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2027</v>
       </c>
@@ -678,7 +779,7 @@
         <v>670457.39348370919</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2028</v>
       </c>
@@ -687,7 +788,7 @@
         <v>651566.41604010016</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2029</v>
       </c>
@@ -696,7 +797,7 @@
         <v>632675.43859649112</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2030</v>
       </c>
@@ -705,7 +806,7 @@
         <v>613784.46115288208</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2031</v>
       </c>
@@ -714,7 +815,7 @@
         <v>594893.48370927304</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2032</v>
       </c>
@@ -723,7 +824,7 @@
         <v>576002.50626566401</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2033</v>
       </c>
@@ -732,7 +833,7 @@
         <v>557111.52882205497</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2034</v>
       </c>
@@ -741,7 +842,7 @@
         <v>538220.55137844593</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2035</v>
       </c>
@@ -750,7 +851,7 @@
         <v>519329.5739348369</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2036</v>
       </c>
@@ -759,7 +860,7 @@
         <v>500438.59649122786</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2037</v>
       </c>
@@ -768,7 +869,7 @@
         <v>481547.61904761882</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2038</v>
       </c>
@@ -777,7 +878,7 @@
         <v>462656.64160400978</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2039</v>
       </c>
@@ -786,7 +887,7 @@
         <v>443765.66416040075</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2040</v>
       </c>
@@ -795,7 +896,7 @@
         <v>424874.68671679171</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2041</v>
       </c>
@@ -804,7 +905,7 @@
         <v>405983.70927318267</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2042</v>
       </c>
@@ -813,7 +914,7 @@
         <v>387092.73182957363</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2043</v>
       </c>
@@ -822,7 +923,7 @@
         <v>368201.7543859646</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2044</v>
       </c>
@@ -831,7 +932,7 @@
         <v>349310.77694235556</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2045</v>
       </c>
@@ -840,7 +941,7 @@
         <v>330419.79949874652</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2046</v>
       </c>
@@ -849,7 +950,7 @@
         <v>311528.82205513748</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2047</v>
       </c>
@@ -858,7 +959,7 @@
         <v>292637.84461152845</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2048</v>
       </c>
@@ -867,7 +968,7 @@
         <v>273746.86716791941</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2049</v>
       </c>
@@ -876,7 +977,7 @@
         <v>254855.8897243104</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2050</v>
       </c>
@@ -884,7 +985,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2051</v>
       </c>
@@ -892,7 +993,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2052</v>
       </c>
@@ -900,7 +1001,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2053</v>
       </c>
@@ -908,7 +1009,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2054</v>
       </c>
@@ -916,7 +1017,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2055</v>
       </c>
@@ -924,7 +1025,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2056</v>
       </c>
@@ -932,7 +1033,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2057</v>
       </c>
@@ -940,7 +1041,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2058</v>
       </c>
@@ -948,7 +1049,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2059</v>
       </c>
@@ -956,7 +1057,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2060</v>
       </c>
@@ -964,7 +1065,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2061</v>
       </c>
@@ -972,7 +1073,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2062</v>
       </c>
@@ -980,7 +1081,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2063</v>
       </c>
@@ -988,7 +1089,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2064</v>
       </c>
@@ -996,7 +1097,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2065</v>
       </c>
@@ -1004,7 +1105,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2066</v>
       </c>
@@ -1012,7 +1113,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2067</v>
       </c>
@@ -1020,7 +1121,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2068</v>
       </c>
@@ -1028,7 +1129,7 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2069</v>
       </c>
@@ -1036,12 +1137,923 @@
         <v>235964.91228070177</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2070</v>
       </c>
       <c r="B82">
         <v>235964.91228070177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FE451C-2A7F-485A-A17C-11DA701185FE}">
+  <dimension ref="A1:C82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1990</v>
+      </c>
+      <c r="B2">
+        <v>934005</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1991</v>
+      </c>
+      <c r="B3">
+        <v>934005</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1992</v>
+      </c>
+      <c r="B4">
+        <v>934005</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1993</v>
+      </c>
+      <c r="B5">
+        <v>934005</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1994</v>
+      </c>
+      <c r="B6">
+        <v>934005</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1995</v>
+      </c>
+      <c r="B7">
+        <v>934005</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1996</v>
+      </c>
+      <c r="B8">
+        <v>934005</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1997</v>
+      </c>
+      <c r="B9">
+        <v>934005</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1998</v>
+      </c>
+      <c r="B10">
+        <v>934005</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1999</v>
+      </c>
+      <c r="B11">
+        <v>934005</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2000</v>
+      </c>
+      <c r="B12">
+        <v>934005</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2001</v>
+      </c>
+      <c r="B13">
+        <v>934005</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2002</v>
+      </c>
+      <c r="B14">
+        <v>934005</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2003</v>
+      </c>
+      <c r="B15">
+        <v>934005</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2004</v>
+      </c>
+      <c r="B16">
+        <v>934005</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2005</v>
+      </c>
+      <c r="B17">
+        <v>934005</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2006</v>
+      </c>
+      <c r="B18">
+        <v>934005</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2007</v>
+      </c>
+      <c r="B19">
+        <v>934005</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2008</v>
+      </c>
+      <c r="B20">
+        <v>934005</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2009</v>
+      </c>
+      <c r="B21">
+        <v>934005</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2010</v>
+      </c>
+      <c r="B22">
+        <v>934005</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2011</v>
+      </c>
+      <c r="B23">
+        <v>934005</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2012</v>
+      </c>
+      <c r="B24">
+        <v>934005</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2013</v>
+      </c>
+      <c r="B25">
+        <v>934005</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2014</v>
+      </c>
+      <c r="B26">
+        <v>934005</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2015</v>
+      </c>
+      <c r="B27">
+        <v>934005</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2016</v>
+      </c>
+      <c r="B28">
+        <v>934005</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2017</v>
+      </c>
+      <c r="B29">
+        <v>934005</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2018</v>
+      </c>
+      <c r="B30">
+        <v>934005</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2019</v>
+      </c>
+      <c r="B31">
+        <v>934005</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2020</v>
+      </c>
+      <c r="B32">
+        <v>934005</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2021</v>
+      </c>
+      <c r="B33" s="1">
+        <v>914546.5625</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2022</v>
+      </c>
+      <c r="B34">
+        <v>895088.125</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2023</v>
+      </c>
+      <c r="B35">
+        <v>875629.6875</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2024</v>
+      </c>
+      <c r="B36">
+        <v>817254.375</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2025</v>
+      </c>
+      <c r="B37">
+        <v>700503.75</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2026</v>
+      </c>
+      <c r="B38">
+        <v>700503.75</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2027</v>
+      </c>
+      <c r="B39">
+        <v>700503.75</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2028</v>
+      </c>
+      <c r="B40">
+        <v>700503.75</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2029</v>
+      </c>
+      <c r="B41">
+        <v>700503.75</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2030</v>
+      </c>
+      <c r="B42">
+        <v>700503.75</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2031</v>
+      </c>
+      <c r="B43">
+        <v>700503.75</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2032</v>
+      </c>
+      <c r="B44">
+        <v>700503.75</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2033</v>
+      </c>
+      <c r="B45">
+        <v>700503.75</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2034</v>
+      </c>
+      <c r="B46">
+        <v>700503.75</v>
+      </c>
+      <c r="C46" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2035</v>
+      </c>
+      <c r="B47">
+        <v>700503.75</v>
+      </c>
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2036</v>
+      </c>
+      <c r="B48">
+        <v>700503.75</v>
+      </c>
+      <c r="C48" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2037</v>
+      </c>
+      <c r="B49">
+        <v>700503.75</v>
+      </c>
+      <c r="C49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2038</v>
+      </c>
+      <c r="B50">
+        <v>700503.75</v>
+      </c>
+      <c r="C50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2039</v>
+      </c>
+      <c r="B51">
+        <v>700503.75</v>
+      </c>
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2040</v>
+      </c>
+      <c r="B52">
+        <v>700503.75</v>
+      </c>
+      <c r="C52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2041</v>
+      </c>
+      <c r="B53">
+        <v>700503.75</v>
+      </c>
+      <c r="C53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2042</v>
+      </c>
+      <c r="B54">
+        <v>700503.75</v>
+      </c>
+      <c r="C54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2043</v>
+      </c>
+      <c r="B55">
+        <v>700503.75</v>
+      </c>
+      <c r="C55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2044</v>
+      </c>
+      <c r="B56">
+        <v>700503.75</v>
+      </c>
+      <c r="C56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2045</v>
+      </c>
+      <c r="B57">
+        <v>700503.75</v>
+      </c>
+      <c r="C57" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2046</v>
+      </c>
+      <c r="B58">
+        <v>700503.75</v>
+      </c>
+      <c r="C58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2047</v>
+      </c>
+      <c r="B59">
+        <v>700503.75</v>
+      </c>
+      <c r="C59" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2048</v>
+      </c>
+      <c r="B60">
+        <v>700503.75</v>
+      </c>
+      <c r="C60" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>2049</v>
+      </c>
+      <c r="B61">
+        <v>700503.75</v>
+      </c>
+      <c r="C61" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2050</v>
+      </c>
+      <c r="B62">
+        <v>700503.75</v>
+      </c>
+      <c r="C62" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2051</v>
+      </c>
+      <c r="B63">
+        <v>700503.75</v>
+      </c>
+      <c r="C63" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2052</v>
+      </c>
+      <c r="B64">
+        <v>700503.75</v>
+      </c>
+      <c r="C64" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2053</v>
+      </c>
+      <c r="B65">
+        <v>700503.75</v>
+      </c>
+      <c r="C65" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2054</v>
+      </c>
+      <c r="B66">
+        <v>700503.75</v>
+      </c>
+      <c r="C66" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2055</v>
+      </c>
+      <c r="B67">
+        <v>700503.75</v>
+      </c>
+      <c r="C67" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2056</v>
+      </c>
+      <c r="B68">
+        <v>700503.75</v>
+      </c>
+      <c r="C68" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2057</v>
+      </c>
+      <c r="B69">
+        <v>700503.75</v>
+      </c>
+      <c r="C69" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2058</v>
+      </c>
+      <c r="B70">
+        <v>700503.75</v>
+      </c>
+      <c r="C70" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2059</v>
+      </c>
+      <c r="B71">
+        <v>700503.75</v>
+      </c>
+      <c r="C71" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2060</v>
+      </c>
+      <c r="B72">
+        <v>700503.75</v>
+      </c>
+      <c r="C72" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2061</v>
+      </c>
+      <c r="B73">
+        <v>700503.75</v>
+      </c>
+      <c r="C73" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2062</v>
+      </c>
+      <c r="B74">
+        <v>700503.75</v>
+      </c>
+      <c r="C74" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2063</v>
+      </c>
+      <c r="B75">
+        <v>700503.75</v>
+      </c>
+      <c r="C75" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2064</v>
+      </c>
+      <c r="B76">
+        <v>700503.75</v>
+      </c>
+      <c r="C76" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2065</v>
+      </c>
+      <c r="B77">
+        <v>700503.75</v>
+      </c>
+      <c r="C77" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>2066</v>
+      </c>
+      <c r="B78">
+        <v>700503.75</v>
+      </c>
+      <c r="C78" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2067</v>
+      </c>
+      <c r="B79">
+        <v>700503.75</v>
+      </c>
+      <c r="C79" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2068</v>
+      </c>
+      <c r="B80">
+        <v>700503.75</v>
+      </c>
+      <c r="C80" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2069</v>
+      </c>
+      <c r="B81">
+        <v>700503.75</v>
+      </c>
+      <c r="C81" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>2070</v>
+      </c>
+      <c r="B82">
+        <v>700503.75</v>
+      </c>
+      <c r="C82" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>